<commit_message>
modification of graphs on iterations
</commit_message>
<xml_diff>
--- a/iterations vs error graphs.xlsx
+++ b/iterations vs error graphs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lambe\Desktop\COMP551\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{080258A9-9CB8-4872-BBBE-CD0272287B51}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{514E45A5-E27D-42B7-94B0-EADFDE3945FD}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14595" xr2:uid="{798E7619-3329-46AF-8A99-A02B20450A3E}"/>
   </bookViews>
@@ -108,67 +108,7 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-CA"/>
-              <a:t>Error</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="en-CA" baseline="0"/>
-              <a:t> descent with higher num of iterations</a:t>
-            </a:r>
-            <a:endParaRPr lang="en-CA"/>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
+    <c:autoTitleDeleted val="1"/>
     <c:plotArea>
       <c:layout>
         <c:manualLayout>
@@ -510,6 +450,7 @@
         <c:axId val="486975392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="0.57000000000000006"/>
           <c:min val="0.27"/>
         </c:scaling>
         <c:delete val="0"/>
@@ -695,64 +636,7 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-CA" sz="1200" b="0" i="0" baseline="0">
-                <a:effectLst/>
-              </a:rPr>
-              <a:t>Error descent with higher num of iterations, fixed learning rate</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
+    <c:autoTitleDeleted val="1"/>
     <c:plotArea>
       <c:layout/>
       <c:scatterChart>
@@ -1054,7 +938,8 @@
         <c:axId val="596330592"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:min val="0.29000000000000004"/>
+          <c:max val="0.42000000000000004"/>
+          <c:min val="0.29500000000000004"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -2709,7 +2594,7 @@
   <dimension ref="A1:N28"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="L28" sqref="L28"/>
+      <selection activeCell="L30" sqref="L30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>

</xml_diff>